<commit_message>
ITST-21306: xlsx-reader: Improve skipEmptyCells handling
- Improve SkipEmptyCellsTest to cover more cases.
- Remove dead code from next().
</commit_message>
<xml_diff>
--- a/tests/input_files/iterator_test.xlsx
+++ b/tests/input_files/iterator_test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t xml:space="preserve">text1</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t xml:space="preserve">Not empty #5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row3, cell2</t>
   </si>
 </sst>
 </file>
@@ -643,7 +646,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
@@ -671,6 +674,11 @@
         <v>22</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>